<commit_message>
implementacion de filtro por cliente y sucursal en dashboar envios
</commit_message>
<xml_diff>
--- a/Files/Temp_os_adm/900987412_3.xlsx
+++ b/Files/Temp_os_adm/900987412_3.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
   <si>
     <t>Nombre Destinatario</t>
   </si>
@@ -197,259 +197,178 @@
     <t>MASLOGISTICA - FLEX</t>
   </si>
   <si>
-    <t>5D</t>
-  </si>
-  <si>
-    <t>8D</t>
-  </si>
-  <si>
-    <t>XDSG0036</t>
-  </si>
-  <si>
-    <t>6D</t>
-  </si>
-  <si>
-    <t>XDXI0008</t>
-  </si>
-  <si>
-    <t>ADSG0021</t>
-  </si>
-  <si>
-    <t>3H</t>
-  </si>
-  <si>
     <t>BOGOTA</t>
   </si>
   <si>
-    <t>ACCESORIOS DE CELULAR</t>
-  </si>
-  <si>
-    <t>Cesar castellanos</t>
-  </si>
-  <si>
-    <t>Calle 180 Bis #16 58-SN</t>
-  </si>
-  <si>
-    <t>065CS25126+065GL24540</t>
-  </si>
-  <si>
-    <t>5B+10F</t>
-  </si>
-  <si>
-    <t>diego rocha</t>
-  </si>
-  <si>
-    <t>179 #6-29</t>
-  </si>
-  <si>
-    <t>wilson javier rodriguez gomez</t>
-  </si>
-  <si>
-    <t>Cra 17 #152-13</t>
-  </si>
-  <si>
-    <t>ACS00438</t>
-  </si>
-  <si>
-    <t>9A</t>
-  </si>
-  <si>
-    <t>: Diana Carolina Barreto Navarro</t>
-  </si>
-  <si>
-    <t>Carrera 69 F #63 C-49</t>
-  </si>
-  <si>
-    <t>ESSG0001</t>
-  </si>
-  <si>
-    <t>1F</t>
-  </si>
-  <si>
-    <t>: Daniel Felipe</t>
-  </si>
-  <si>
-    <t>calle29A#1A11este barrio cordoba</t>
-  </si>
-  <si>
-    <t>FXXI0018</t>
-  </si>
-  <si>
-    <t>Juan Gómez</t>
-  </si>
-  <si>
-    <t>Carrera 79a #5-54sur</t>
-  </si>
-  <si>
-    <t>ASD00261</t>
-  </si>
-  <si>
     <t>5B</t>
   </si>
   <si>
-    <t>Sergio Cruz</t>
-  </si>
-  <si>
-    <t>Calle 57A #35A-30</t>
-  </si>
-  <si>
-    <t>000GL21813+042GL20423</t>
-  </si>
-  <si>
-    <t>10F+10E</t>
-  </si>
-  <si>
-    <t>John Gregory Parra Puentes</t>
-  </si>
-  <si>
-    <t>Cra. 50 B. #64-44</t>
-  </si>
-  <si>
-    <t>XDXI0017</t>
-  </si>
-  <si>
-    <t>Yeison Martinez Casas</t>
-  </si>
-  <si>
-    <t>Diagonal 73g sur #78d-75</t>
-  </si>
-  <si>
-    <t>ASD00993</t>
-  </si>
-  <si>
-    <t>2B</t>
-  </si>
-  <si>
-    <t>NAZLY CADENA</t>
-  </si>
-  <si>
-    <t>Diagonal 61D #24-46</t>
-  </si>
-  <si>
-    <t>FSSG0058</t>
-  </si>
-  <si>
-    <t>9C</t>
-  </si>
-  <si>
-    <t>Tomas Reines</t>
-  </si>
-  <si>
-    <t>Carrera 17 #106-52</t>
-  </si>
-  <si>
-    <t>ACEC0010</t>
-  </si>
-  <si>
-    <t>6B</t>
-  </si>
-  <si>
-    <t>JULIAN ORDUZ</t>
-  </si>
-  <si>
-    <t>Calle 161 #54-25</t>
-  </si>
-  <si>
-    <t>ACEC0011</t>
-  </si>
-  <si>
-    <t>Augusto Velasquez</t>
-  </si>
-  <si>
-    <t>Calle 23 # 68-59 Torre 14 Apto 401</t>
-  </si>
-  <si>
-    <t>Julio Manrique</t>
-  </si>
-  <si>
-    <t>: carrera 45 #61-10</t>
-  </si>
-  <si>
-    <t>ACH02022</t>
-  </si>
-  <si>
-    <t>11E</t>
-  </si>
-  <si>
-    <t>Lina Ramirez</t>
-  </si>
-  <si>
-    <t>carrera 75 #167-89</t>
-  </si>
-  <si>
-    <t>EF-ZN980CBEGUS</t>
-  </si>
-  <si>
     <t>1A</t>
   </si>
   <si>
-    <t>David Andrés Rodriguez</t>
-  </si>
-  <si>
-    <t>Calle 70D Bis #113A-17</t>
-  </si>
-  <si>
-    <t>EP-DG950CBE-BULK</t>
-  </si>
-  <si>
-    <t>11D</t>
-  </si>
-  <si>
-    <t>Nicolás París Riaño</t>
-  </si>
-  <si>
-    <t>Carrera 50 #102-38</t>
-  </si>
-  <si>
-    <t>ACEC0013</t>
-  </si>
-  <si>
-    <t>4B</t>
-  </si>
-  <si>
-    <t>Jose Pablo Uribe Lopez</t>
-  </si>
-  <si>
-    <t>Calle 125 #70F-49</t>
-  </si>
-  <si>
-    <t>FUSG0059</t>
-  </si>
-  <si>
-    <t>7D</t>
-  </si>
-  <si>
-    <t>ANGELA ALDANA</t>
-  </si>
-  <si>
-    <t>carrera 136A #145-30</t>
-  </si>
-  <si>
-    <t>Francisco Javier Franco Posada</t>
-  </si>
-  <si>
-    <t>Carrera 14B #148-10</t>
-  </si>
-  <si>
-    <t>FUSG0052+DWSG0008</t>
-  </si>
-  <si>
-    <t>7C+3E</t>
-  </si>
-  <si>
-    <t>Helmuth Garcia Peter</t>
-  </si>
-  <si>
-    <t>Calle 103 #17A-28</t>
-  </si>
-  <si>
-    <t>ivan arturo salazar</t>
-  </si>
-  <si>
-    <t>Carrera 2a #66-52</t>
-  </si>
-  <si>
-    <t>Calle 151 #111a-87</t>
+    <t>FXXI0020</t>
+  </si>
+  <si>
+    <t>6E</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>TA50-BLANCO</t>
+  </si>
+  <si>
+    <t>11F</t>
+  </si>
+  <si>
+    <t>7F</t>
+  </si>
+  <si>
+    <t>FUSG0019</t>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>FXHW0020</t>
+  </si>
+  <si>
+    <t>ACS01306</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>ACCESORIOS CELULAR</t>
+  </si>
+  <si>
+    <t>ASD01277</t>
+  </si>
+  <si>
+    <t>10D</t>
+  </si>
+  <si>
+    <t>BASG0009</t>
+  </si>
+  <si>
+    <t>Melissa Marquez</t>
+  </si>
+  <si>
+    <t>Calle 6d Este #4-32</t>
+  </si>
+  <si>
+    <t>Damiano Nocera</t>
+  </si>
+  <si>
+    <t>Carrera 16 #106-45</t>
+  </si>
+  <si>
+    <t>Victor Fernando Moreno</t>
+  </si>
+  <si>
+    <t>Diagonal 82 bis #85 -21</t>
+  </si>
+  <si>
+    <t>Jenny Niño</t>
+  </si>
+  <si>
+    <t>Calle 164 #14A-25</t>
+  </si>
+  <si>
+    <t>ASD00840</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>avid gonzalez</t>
+  </si>
+  <si>
+    <t>carrera 4 #69-45</t>
+  </si>
+  <si>
+    <t>062CS24469</t>
+  </si>
+  <si>
+    <t>Jhaniat Azuaje</t>
+  </si>
+  <si>
+    <t>Calle 134A #10A-11</t>
+  </si>
+  <si>
+    <t>DWHW0003</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>Tatiana Orozco</t>
+  </si>
+  <si>
+    <t>Carrera 18c #122-40</t>
+  </si>
+  <si>
+    <t>XDAP0008</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>jaime gonzalez</t>
+  </si>
+  <si>
+    <t>calle 100 #53-48</t>
+  </si>
+  <si>
+    <t>Alejandra Acevedo</t>
+  </si>
+  <si>
+    <t>Diagonal 13 Bis sur #24D-42</t>
+  </si>
+  <si>
+    <t>XMAP0006</t>
+  </si>
+  <si>
+    <t>Juan Camilo Ordoñez</t>
+  </si>
+  <si>
+    <t>Calle 49 #6-39</t>
+  </si>
+  <si>
+    <t>Hamilton Espitia</t>
+  </si>
+  <si>
+    <t>Calle 6A # 88D - 71</t>
+  </si>
+  <si>
+    <t>Juan Valen</t>
+  </si>
+  <si>
+    <t>Carrera 118A #22D-36</t>
+  </si>
+  <si>
+    <t>Erick Espejo Silva</t>
+  </si>
+  <si>
+    <t>Calle 127 bis #88-07</t>
+  </si>
+  <si>
+    <t>karen Florez</t>
+  </si>
+  <si>
+    <t>carrera 75 #150-50</t>
+  </si>
+  <si>
+    <t>Pablo Montes</t>
+  </si>
+  <si>
+    <t>Calle 181 #18B-82</t>
+  </si>
+  <si>
+    <t>Nicolas Hernandez</t>
+  </si>
+  <si>
+    <t>Calle 160 No.57-70 apto 703 torre 2 Balcones de la colina</t>
   </si>
 </sst>
 </file>
@@ -867,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="G2" sqref="G2:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,462 +832,328 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40307381272</v>
+        <v>40315156408</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2">
+        <v>3106337436</v>
+      </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40305249480</v>
+        <v>40315114071</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
+      <c r="F3">
+        <v>3157575573</v>
+      </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40307254379</v>
+        <v>40315024036</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40307171957</v>
+        <v>40314885563</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40307120575</v>
+        <v>40314833930</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40306971671</v>
+        <v>40314781999</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40307064155</v>
+        <v>40314411075</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40306978156</v>
+        <v>40314368295</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40306704147</v>
+        <v>40314237213</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40306684940</v>
+        <v>40314076292</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40306552224</v>
+        <v>40316043102</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40306543911</v>
+        <v>40316002591</v>
       </c>
       <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40306540101</v>
+        <v>40315975861</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>40306194554</v>
+        <v>40315873981</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>40306175656</v>
+        <v>40315846102</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>40306081514</v>
+        <v>100008305</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>40306019879</v>
-      </c>
-      <c r="B18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>40306003323</v>
-      </c>
-      <c r="B19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>40305794496</v>
-      </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>40307540105</v>
-      </c>
-      <c r="B21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>40307490160</v>
-      </c>
-      <c r="B22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>40307440340</v>
-      </c>
-      <c r="B23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>40307414971</v>
-      </c>
-      <c r="B24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1380,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I24"/>
+      <selection activeCell="I2" sqref="I2:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,18 +1181,18 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40307381272</v>
+        <v>40315156408</v>
       </c>
       <c r="B2">
-        <v>4259563459</v>
+        <v>4268343865</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1416,27 +1201,30 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2">
+        <v>40315156408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>40315114071</v>
+      </c>
+      <c r="B3">
+        <v>4268298165</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>40305249480</v>
-      </c>
-      <c r="B3">
-        <v>4257147790</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1445,27 +1233,30 @@
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="J3">
+        <v>40315114071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40307254379</v>
+        <v>40315024036</v>
       </c>
       <c r="B4">
-        <v>4259420155</v>
+        <v>4268191532</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1474,27 +1265,30 @@
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>40315024036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40307171957</v>
+        <v>40314885563</v>
       </c>
       <c r="B5">
-        <v>4259325170</v>
+        <v>4268029994</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1503,56 +1297,62 @@
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="J5">
+        <v>40314885563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40307120575</v>
+        <v>40314833930</v>
       </c>
       <c r="B6">
-        <v>4259265534</v>
+        <v>4267971772</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="J6">
+        <v>40314833930</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40306971671</v>
+        <v>40314781999</v>
       </c>
       <c r="B7">
-        <v>4259093829</v>
+        <v>4267918121</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1561,27 +1361,30 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="J7">
+        <v>40314781999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40307064155</v>
+        <v>40314411075</v>
       </c>
       <c r="B8">
-        <v>4259203064</v>
+        <v>4267497606</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1590,27 +1393,30 @@
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="J8">
+        <v>40314411075</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40306978156</v>
+        <v>40314368295</v>
       </c>
       <c r="B9">
-        <v>4259098530</v>
+        <v>4267450561</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1619,27 +1425,30 @@
         <v>9</v>
       </c>
       <c r="F9" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <v>40314368295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40306704147</v>
+        <v>40314237213</v>
       </c>
       <c r="B10">
-        <v>4258793659</v>
+        <v>4267302447</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1648,27 +1457,30 @@
         <v>9</v>
       </c>
       <c r="F10" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="J10">
+        <v>40314237213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40306684940</v>
+        <v>40314076292</v>
       </c>
       <c r="B11">
-        <v>4258771649</v>
+        <v>4267117884</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1677,27 +1489,30 @@
         <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J11">
+        <v>40314076292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40306552224</v>
+        <v>40316043102</v>
       </c>
       <c r="B12">
-        <v>4258621834</v>
+        <v>4269349574</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1706,27 +1521,30 @@
         <v>9</v>
       </c>
       <c r="F12" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="J12">
+        <v>40316043102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40306543911</v>
+        <v>40316002591</v>
       </c>
       <c r="B13">
-        <v>4258615009</v>
+        <v>4269306174</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1735,27 +1553,30 @@
         <v>9</v>
       </c>
       <c r="F13" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
         <v>58</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>59</v>
       </c>
-      <c r="I13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>40316002591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40306540101</v>
+        <v>40315975861</v>
       </c>
       <c r="B14">
-        <v>4258610138</v>
+        <v>4269271886</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1764,27 +1585,30 @@
         <v>9</v>
       </c>
       <c r="F14" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="J14">
+        <v>40315975861</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>40306194554</v>
+        <v>40315873981</v>
       </c>
       <c r="B15">
-        <v>4258222342</v>
+        <v>4269156941</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1793,27 +1617,30 @@
         <v>9</v>
       </c>
       <c r="F15" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="J15">
+        <v>40315873981</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>40306175656</v>
+        <v>40315846102</v>
       </c>
       <c r="B16">
-        <v>4258198757</v>
+        <v>4269129202</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1822,27 +1649,30 @@
         <v>9</v>
       </c>
       <c r="F16" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="J16">
+        <v>40315846102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>40306081514</v>
+        <v>100008305</v>
       </c>
       <c r="B17">
-        <v>4258093911</v>
+        <v>1767</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1851,220 +1681,164 @@
         <v>9</v>
       </c>
       <c r="F17" s="3">
-        <v>44188</v>
+        <v>44194</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>40306019879</v>
-      </c>
-      <c r="B18">
-        <v>4258022931</v>
-      </c>
-      <c r="C18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="3">
-        <v>44188</v>
-      </c>
-      <c r="G18" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>40306003323</v>
-      </c>
-      <c r="B19">
-        <v>4258005919</v>
-      </c>
-      <c r="C19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="3">
-        <v>44188</v>
-      </c>
-      <c r="G19" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>40305794496</v>
-      </c>
-      <c r="B20">
-        <v>4257771399</v>
-      </c>
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="3">
-        <v>44188</v>
-      </c>
-      <c r="G20" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" t="s">
-        <v>84</v>
-      </c>
-      <c r="I20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>40307540105</v>
-      </c>
-      <c r="B21">
-        <v>40307540105</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="3">
-        <v>44188</v>
-      </c>
-      <c r="G21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" t="s">
-        <v>86</v>
-      </c>
-      <c r="I21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>40307490160</v>
-      </c>
-      <c r="B22">
-        <v>4259684824</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="3">
-        <v>44188</v>
-      </c>
-      <c r="G22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>40307440340</v>
-      </c>
-      <c r="B23">
-        <v>4259627851</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="3">
-        <v>44188</v>
-      </c>
-      <c r="G23" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>40307414971</v>
-      </c>
-      <c r="B24">
-        <v>4259605014</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="3">
-        <v>44188</v>
-      </c>
-      <c r="G24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" t="s">
-        <v>94</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="J17">
+        <v>100008305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implementacion de filtro por sucursal en dashboard envios vista cliente
</commit_message>
<xml_diff>
--- a/Files/Temp_os_adm/900987412_3.xlsx
+++ b/Files/Temp_os_adm/900987412_3.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
   <si>
     <t>Nombre Destinatario</t>
   </si>
@@ -203,172 +203,157 @@
     <t>5B</t>
   </si>
   <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>FXXI0020</t>
-  </si>
-  <si>
     <t>6E</t>
   </si>
   <si>
-    <t>1C</t>
-  </si>
-  <si>
-    <t>TA50-BLANCO</t>
-  </si>
-  <si>
     <t>11F</t>
   </si>
   <si>
+    <t>10F</t>
+  </si>
+  <si>
+    <t>3F</t>
+  </si>
+  <si>
     <t>7F</t>
   </si>
   <si>
-    <t>FUSG0019</t>
-  </si>
-  <si>
-    <t>2H</t>
-  </si>
-  <si>
-    <t>FXHW0020</t>
-  </si>
-  <si>
-    <t>ACS01306</t>
-  </si>
-  <si>
-    <t>9B</t>
+    <t>3G</t>
+  </si>
+  <si>
+    <t>076CS27184</t>
+  </si>
+  <si>
+    <t>4D</t>
   </si>
   <si>
     <t>ACCESORIOS CELULAR</t>
   </si>
   <si>
-    <t>ASD01277</t>
-  </si>
-  <si>
-    <t>10D</t>
-  </si>
-  <si>
-    <t>BASG0009</t>
-  </si>
-  <si>
-    <t>Melissa Marquez</t>
-  </si>
-  <si>
-    <t>Calle 6d Este #4-32</t>
-  </si>
-  <si>
-    <t>Damiano Nocera</t>
-  </si>
-  <si>
-    <t>Carrera 16 #106-45</t>
-  </si>
-  <si>
-    <t>Victor Fernando Moreno</t>
-  </si>
-  <si>
-    <t>Diagonal 82 bis #85 -21</t>
-  </si>
-  <si>
-    <t>Jenny Niño</t>
-  </si>
-  <si>
-    <t>Calle 164 #14A-25</t>
-  </si>
-  <si>
-    <t>ASD00840</t>
-  </si>
-  <si>
-    <t>1B</t>
-  </si>
-  <si>
-    <t>avid gonzalez</t>
-  </si>
-  <si>
-    <t>carrera 4 #69-45</t>
-  </si>
-  <si>
-    <t>062CS24469</t>
-  </si>
-  <si>
-    <t>Jhaniat Azuaje</t>
-  </si>
-  <si>
-    <t>Calle 134A #10A-11</t>
-  </si>
-  <si>
-    <t>DWHW0003</t>
-  </si>
-  <si>
-    <t>1D</t>
-  </si>
-  <si>
-    <t>Tatiana Orozco</t>
-  </si>
-  <si>
-    <t>Carrera 18c #122-40</t>
-  </si>
-  <si>
-    <t>XDAP0008</t>
-  </si>
-  <si>
-    <t>2C</t>
-  </si>
-  <si>
-    <t>jaime gonzalez</t>
-  </si>
-  <si>
-    <t>calle 100 #53-48</t>
-  </si>
-  <si>
-    <t>Alejandra Acevedo</t>
-  </si>
-  <si>
-    <t>Diagonal 13 Bis sur #24D-42</t>
-  </si>
-  <si>
-    <t>XMAP0006</t>
-  </si>
-  <si>
-    <t>Juan Camilo Ordoñez</t>
-  </si>
-  <si>
-    <t>Calle 49 #6-39</t>
-  </si>
-  <si>
-    <t>Hamilton Espitia</t>
-  </si>
-  <si>
-    <t>Calle 6A # 88D - 71</t>
-  </si>
-  <si>
-    <t>Juan Valen</t>
-  </si>
-  <si>
-    <t>Carrera 118A #22D-36</t>
-  </si>
-  <si>
-    <t>Erick Espejo Silva</t>
-  </si>
-  <si>
-    <t>Calle 127 bis #88-07</t>
-  </si>
-  <si>
-    <t>karen Florez</t>
-  </si>
-  <si>
-    <t>carrera 75 #150-50</t>
-  </si>
-  <si>
-    <t>Pablo Montes</t>
-  </si>
-  <si>
-    <t>Calle 181 #18B-82</t>
-  </si>
-  <si>
-    <t>Nicolas Hernandez</t>
-  </si>
-  <si>
-    <t>Calle 160 No.57-70 apto 703 torre 2 Balcones de la colina</t>
+    <t>ASD00993</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>Sebastián Triana</t>
+  </si>
+  <si>
+    <t>Carrera 68f #96-40</t>
+  </si>
+  <si>
+    <t>FXXI0005</t>
+  </si>
+  <si>
+    <t>Mairly Giraldo</t>
+  </si>
+  <si>
+    <t>Calle 38g sur #68c-63</t>
+  </si>
+  <si>
+    <t>FXXI0010</t>
+  </si>
+  <si>
+    <t>8F</t>
+  </si>
+  <si>
+    <t>Orlando Bustamante</t>
+  </si>
+  <si>
+    <t>calle 22B #44A-33</t>
+  </si>
+  <si>
+    <t>FXXI0004</t>
+  </si>
+  <si>
+    <t>ANDRES CAMACHO</t>
+  </si>
+  <si>
+    <t>Cra 5c #48J-82sur</t>
+  </si>
+  <si>
+    <t>ESSG0008</t>
+  </si>
+  <si>
+    <t>nicolas cruz</t>
+  </si>
+  <si>
+    <t>Transversal 13 C este #48a-09s</t>
+  </si>
+  <si>
+    <t>XDXI0011</t>
+  </si>
+  <si>
+    <t>Sergio Hernández</t>
+  </si>
+  <si>
+    <t>Calle 57B Sur #62-13</t>
+  </si>
+  <si>
+    <t>AGL01533</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>ingrid yadira espitia castañeda</t>
+  </si>
+  <si>
+    <t>Calle 86a #69t-81</t>
+  </si>
+  <si>
+    <t>leonardo hoyos</t>
+  </si>
+  <si>
+    <t>Cra 73B #64F-58</t>
+  </si>
+  <si>
+    <t>ASD00841</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>Camilo Cuervo Díaz</t>
+  </si>
+  <si>
+    <t>Transversal 19A #95-56</t>
+  </si>
+  <si>
+    <t>ST75874RS</t>
+  </si>
+  <si>
+    <t>STIVEN GORDILLO MURCIA</t>
+  </si>
+  <si>
+    <t>Diagonal 2A #79F-26</t>
+  </si>
+  <si>
+    <t>ACSG0001</t>
+  </si>
+  <si>
+    <t>Camilo Romero</t>
+  </si>
+  <si>
+    <t>Carrera 3 #74A-50</t>
+  </si>
+  <si>
+    <t>XDHW0004</t>
+  </si>
+  <si>
+    <t>Francisco Javier Mendez</t>
+  </si>
+  <si>
+    <t>Carrera90 #6a-98</t>
+  </si>
+  <si>
+    <t>XMAP0002</t>
+  </si>
+  <si>
+    <t>BRUCE CASTELLANOS</t>
+  </si>
+  <si>
+    <t>CRA 23D # 2-54 BARRIO LA FRAGÜITA</t>
   </si>
 </sst>
 </file>
@@ -786,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G17"/>
+      <selection activeCell="A15" sqref="A15:XFD114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,13 +817,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40315156408</v>
+        <v>40317700413</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -846,22 +831,19 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>3106337436</v>
-      </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40315114071</v>
+        <v>40317696854</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -869,22 +851,19 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
-        <v>3157575573</v>
-      </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40315024036</v>
+        <v>40317691488</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -893,18 +872,18 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40314885563</v>
+        <v>40317605804</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -913,18 +892,18 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40314833930</v>
+        <v>40317529633</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -933,18 +912,18 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40314781999</v>
+        <v>40317479749</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -953,18 +932,18 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40314411075</v>
+        <v>40316841061</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -973,18 +952,18 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40314368295</v>
+        <v>40316830437</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -993,18 +972,18 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40314237213</v>
+        <v>40316455848</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1013,18 +992,18 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40314076292</v>
+        <v>40316213857</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1033,18 +1012,18 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40316043102</v>
+        <v>40316195365</v>
       </c>
       <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1053,12 +1032,12 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40316002591</v>
+        <v>40316124521</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
@@ -1073,18 +1052,18 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40315975861</v>
+        <v>100008308</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1093,67 +1072,7 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>40315873981</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>40315846102</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>100008305</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1087,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I17"/>
+      <selection activeCell="H2" sqref="H2:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,13 +1105,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40315156408</v>
+        <v>40317700413</v>
       </c>
       <c r="B2">
-        <v>4268343865</v>
+        <v>4271228271</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1201,30 +1120,30 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J2">
-        <v>40315156408</v>
+        <v>40317700413</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40315114071</v>
+        <v>40317696854</v>
       </c>
       <c r="B3">
-        <v>4268298165</v>
+        <v>4271221541</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1233,30 +1152,30 @@
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J3">
-        <v>40315114071</v>
+        <v>40317696854</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40315024036</v>
+        <v>40317691488</v>
       </c>
       <c r="B4">
-        <v>4268191532</v>
+        <v>4271218258</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1265,30 +1184,30 @@
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4">
-        <v>40315024036</v>
+        <v>40317691488</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40314885563</v>
+        <v>40317605804</v>
       </c>
       <c r="B5">
-        <v>4268029994</v>
+        <v>4271119539</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1297,62 +1216,62 @@
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
       <c r="J5">
-        <v>40314885563</v>
+        <v>40317605804</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40314833930</v>
+        <v>40317529633</v>
       </c>
       <c r="B6">
-        <v>4267971772</v>
+        <v>4271032951</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
       <c r="J6">
-        <v>40314833930</v>
+        <v>40317529633</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40314781999</v>
+        <v>40317479749</v>
       </c>
       <c r="B7">
-        <v>4267918121</v>
+        <v>4270978937</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1361,30 +1280,30 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J7">
-        <v>40314781999</v>
+        <v>40317479749</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40314411075</v>
+        <v>40316841061</v>
       </c>
       <c r="B8">
-        <v>4267497606</v>
+        <v>4270248701</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1393,30 +1312,30 @@
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" t="s">
-        <v>46</v>
-      </c>
       <c r="J8">
-        <v>40314411075</v>
+        <v>40316841061</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40314368295</v>
+        <v>40316830437</v>
       </c>
       <c r="B9">
-        <v>4267450561</v>
+        <v>4270240840</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1425,30 +1344,30 @@
         <v>9</v>
       </c>
       <c r="F9" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J9">
-        <v>40314368295</v>
+        <v>40316830437</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40314237213</v>
+        <v>40316455848</v>
       </c>
       <c r="B10">
-        <v>4267302447</v>
+        <v>4269817874</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1457,30 +1376,30 @@
         <v>9</v>
       </c>
       <c r="F10" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J10">
-        <v>40314237213</v>
+        <v>40316455848</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40314076292</v>
+        <v>40316213857</v>
       </c>
       <c r="B11">
-        <v>4267117884</v>
+        <v>4269541997</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1489,30 +1408,30 @@
         <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J11">
-        <v>40314076292</v>
+        <v>40316213857</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40316043102</v>
+        <v>40316195365</v>
       </c>
       <c r="B12">
-        <v>4269349574</v>
+        <v>4269524164</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1521,30 +1440,30 @@
         <v>9</v>
       </c>
       <c r="F12" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
         <v>56</v>
       </c>
-      <c r="I12" t="s">
-        <v>57</v>
-      </c>
       <c r="J12">
-        <v>40316043102</v>
+        <v>40316195365</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40316002591</v>
+        <v>40316124521</v>
       </c>
       <c r="B13">
-        <v>4269306174</v>
+        <v>4269441491</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1553,10 +1472,10 @@
         <v>9</v>
       </c>
       <c r="F13" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
         <v>58</v>
@@ -1565,18 +1484,18 @@
         <v>59</v>
       </c>
       <c r="J13">
-        <v>40316002591</v>
+        <v>40316124521</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40315975861</v>
+        <v>100008308</v>
       </c>
       <c r="B14">
-        <v>4269271886</v>
+        <v>4168110107</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1585,160 +1504,73 @@
         <v>9</v>
       </c>
       <c r="F14" s="3">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J14">
-        <v>40315975861</v>
+        <v>100008308</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>40315873981</v>
-      </c>
-      <c r="B15">
-        <v>4269156941</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="3">
-        <v>44194</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15">
-        <v>40315873981</v>
-      </c>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>40315846102</v>
-      </c>
-      <c r="B16">
-        <v>4269129202</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="3">
-        <v>44194</v>
-      </c>
-      <c r="G16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16">
-        <v>40315846102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>100008305</v>
-      </c>
-      <c r="B17">
-        <v>1767</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="3">
-        <v>44194</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17">
-        <v>100008305</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actualizacion de carga de vistas en panel de administracion
</commit_message>
<xml_diff>
--- a/Files/Temp_os_adm/900987412_3.xlsx
+++ b/Files/Temp_os_adm/900987412_3.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="171">
   <si>
     <t>Nombre Destinatario</t>
   </si>
@@ -215,9 +215,6 @@
     <t>3F</t>
   </si>
   <si>
-    <t>7F</t>
-  </si>
-  <si>
     <t>3G</t>
   </si>
   <si>
@@ -230,130 +227,457 @@
     <t>ACCESORIOS CELULAR</t>
   </si>
   <si>
-    <t>ASD00993</t>
-  </si>
-  <si>
-    <t>2B</t>
-  </si>
-  <si>
-    <t>Sebastián Triana</t>
-  </si>
-  <si>
-    <t>Carrera 68f #96-40</t>
-  </si>
-  <si>
-    <t>FXXI0005</t>
-  </si>
-  <si>
-    <t>Mairly Giraldo</t>
-  </si>
-  <si>
-    <t>Calle 38g sur #68c-63</t>
-  </si>
-  <si>
     <t>FXXI0010</t>
   </si>
   <si>
     <t>8F</t>
   </si>
   <si>
-    <t>Orlando Bustamante</t>
-  </si>
-  <si>
-    <t>calle 22B #44A-33</t>
-  </si>
-  <si>
-    <t>FXXI0004</t>
-  </si>
-  <si>
-    <t>ANDRES CAMACHO</t>
-  </si>
-  <si>
-    <t>Cra 5c #48J-82sur</t>
-  </si>
-  <si>
     <t>ESSG0008</t>
   </si>
   <si>
-    <t>nicolas cruz</t>
-  </si>
-  <si>
-    <t>Transversal 13 C este #48a-09s</t>
-  </si>
-  <si>
-    <t>XDXI0011</t>
-  </si>
-  <si>
-    <t>Sergio Hernández</t>
-  </si>
-  <si>
-    <t>Calle 57B Sur #62-13</t>
-  </si>
-  <si>
-    <t>AGL01533</t>
-  </si>
-  <si>
-    <t>8A</t>
-  </si>
-  <si>
-    <t>ingrid yadira espitia castañeda</t>
-  </si>
-  <si>
-    <t>Calle 86a #69t-81</t>
-  </si>
-  <si>
-    <t>leonardo hoyos</t>
-  </si>
-  <si>
-    <t>Cra 73B #64F-58</t>
-  </si>
-  <si>
     <t>ASD00841</t>
   </si>
   <si>
     <t>5A</t>
   </si>
   <si>
-    <t>Camilo Cuervo Díaz</t>
-  </si>
-  <si>
-    <t>Transversal 19A #95-56</t>
-  </si>
-  <si>
-    <t>ST75874RS</t>
-  </si>
-  <si>
-    <t>STIVEN GORDILLO MURCIA</t>
-  </si>
-  <si>
-    <t>Diagonal 2A #79F-26</t>
-  </si>
-  <si>
-    <t>ACSG0001</t>
-  </si>
-  <si>
-    <t>Camilo Romero</t>
-  </si>
-  <si>
-    <t>Carrera 3 #74A-50</t>
-  </si>
-  <si>
     <t>XDHW0004</t>
   </si>
   <si>
-    <t>Francisco Javier Mendez</t>
-  </si>
-  <si>
-    <t>Carrera90 #6a-98</t>
-  </si>
-  <si>
-    <t>XMAP0002</t>
-  </si>
-  <si>
-    <t>BRUCE CASTELLANOS</t>
-  </si>
-  <si>
-    <t>CRA 23D # 2-54 BARRIO LA FRAGÜITA</t>
+    <t>ACS02159</t>
+  </si>
+  <si>
+    <t>Daniel Cadosch</t>
+  </si>
+  <si>
+    <t>calle 146 #17-88</t>
+  </si>
+  <si>
+    <t>062CS25324</t>
+  </si>
+  <si>
+    <t>11D</t>
+  </si>
+  <si>
+    <t>Tonny Marquez</t>
+  </si>
+  <si>
+    <t>Calle 114a #19a-36</t>
+  </si>
+  <si>
+    <t>DWSG0003</t>
+  </si>
+  <si>
+    <t>10E</t>
+  </si>
+  <si>
+    <t>Laura Pineda</t>
+  </si>
+  <si>
+    <t>Calle 49 #5--34</t>
+  </si>
+  <si>
+    <t>TA50-BLANCO</t>
+  </si>
+  <si>
+    <t>Paola suarez</t>
+  </si>
+  <si>
+    <t>Cra 88c #49c-52sur</t>
+  </si>
+  <si>
+    <t>ACEC0024</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>steven heredia</t>
+  </si>
+  <si>
+    <t>Calle 21 #05-31</t>
+  </si>
+  <si>
+    <t>XDXI0017</t>
+  </si>
+  <si>
+    <t>8D</t>
+  </si>
+  <si>
+    <t>Manuel Fajardo</t>
+  </si>
+  <si>
+    <t>Calle 54 sur #24A-30</t>
+  </si>
+  <si>
+    <t>1F</t>
+  </si>
+  <si>
+    <t>ASD01277</t>
+  </si>
+  <si>
+    <t>10D</t>
+  </si>
+  <si>
+    <t>Francisco Blandon</t>
+  </si>
+  <si>
+    <t>Calle 159 #54-69</t>
+  </si>
+  <si>
+    <t>ASD00261</t>
+  </si>
+  <si>
+    <t>Victor Alfonso Pinzon verdeza</t>
+  </si>
+  <si>
+    <t>Calle 25B #100-55</t>
+  </si>
+  <si>
+    <t>EP-TA20JBEUGUS</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Carlos Santa</t>
+  </si>
+  <si>
+    <t>Carrera 69D #24A-81</t>
+  </si>
+  <si>
+    <t>ADSG0018</t>
+  </si>
+  <si>
+    <t>3H</t>
+  </si>
+  <si>
+    <t>Juliana Ospina</t>
+  </si>
+  <si>
+    <t>Calle 78 #5-50</t>
+  </si>
+  <si>
+    <t>ASD01117</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>Mateo Montañez</t>
+  </si>
+  <si>
+    <t>Carrera 72a #120-31</t>
+  </si>
+  <si>
+    <t>DWSG0005</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>Jefferson Ochoa</t>
+  </si>
+  <si>
+    <t>Cra 59 #94b -43</t>
+  </si>
+  <si>
+    <t>ASD00537</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>Edilberto Lozano Torres</t>
+  </si>
+  <si>
+    <t>Carrera 107 #139-51</t>
+  </si>
+  <si>
+    <t>XDSG0029</t>
+  </si>
+  <si>
+    <t>Ricardo Alberto Morales Navarro</t>
+  </si>
+  <si>
+    <t>Carrera 53g #5A-25</t>
+  </si>
+  <si>
+    <t>DWSG0009</t>
+  </si>
+  <si>
+    <t>Gregorio cordoba</t>
+  </si>
+  <si>
+    <t>Carrera 22 #188-15</t>
+  </si>
+  <si>
+    <t>XDXI0007</t>
+  </si>
+  <si>
+    <t>2G</t>
+  </si>
+  <si>
+    <t>057CS22123</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>Christian Castiblanco</t>
+  </si>
+  <si>
+    <t>Carrera 8 #172 A-85</t>
+  </si>
+  <si>
+    <t>Nancy Margarita Torres Canizales</t>
+  </si>
+  <si>
+    <t>Carrera 17 #106-52-SN</t>
+  </si>
+  <si>
+    <t>062CS24469</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>habib mantilla</t>
+  </si>
+  <si>
+    <t>Carrera 2 #62a-20</t>
+  </si>
+  <si>
+    <t>FXXI0022</t>
+  </si>
+  <si>
+    <t>5D</t>
+  </si>
+  <si>
+    <t>Brigitte Guav</t>
+  </si>
+  <si>
+    <t>Transversal 88 B Sur #73-91</t>
+  </si>
+  <si>
+    <t>5E</t>
+  </si>
+  <si>
+    <t>000GL21813</t>
+  </si>
+  <si>
+    <t>Ricardo Ramírez</t>
+  </si>
+  <si>
+    <t>Calle 143 #9-55</t>
+  </si>
+  <si>
+    <t>XDAP0009</t>
+  </si>
+  <si>
+    <t>David Martínez Ardila</t>
+  </si>
+  <si>
+    <t>Calle 159 #54-78</t>
+  </si>
+  <si>
+    <t>Diego Huertas</t>
+  </si>
+  <si>
+    <t>Transversal 74D #40H-14S</t>
+  </si>
+  <si>
+    <t>XDXI0010</t>
+  </si>
+  <si>
+    <t>JOSE GUILLERMO PEREZ</t>
+  </si>
+  <si>
+    <t>carrera 87D #49C-56</t>
+  </si>
+  <si>
+    <t>ALEXANDER PATIÑO REYES</t>
+  </si>
+  <si>
+    <t>Calle 163A #19A-81</t>
+  </si>
+  <si>
+    <t>FUSG0037</t>
+  </si>
+  <si>
+    <t>Helbert Silva</t>
+  </si>
+  <si>
+    <t>Calle 165B #13C-55</t>
+  </si>
+  <si>
+    <t>Hans Van Strahlen</t>
+  </si>
+  <si>
+    <t>Calle 31a #2a-69</t>
+  </si>
+  <si>
+    <t>Andrea Perdomo Velandia</t>
+  </si>
+  <si>
+    <t>calle 91 #13a-45</t>
+  </si>
+  <si>
+    <t>XDXI0012</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>JUAN CARLOS PALACIOS</t>
+  </si>
+  <si>
+    <t>Cra 15 #161A-48</t>
+  </si>
+  <si>
+    <t>anderzon garzon lozano</t>
+  </si>
+  <si>
+    <t>Cra91b #54 78 sur-SN</t>
+  </si>
+  <si>
+    <t>Diego Alejandro López</t>
+  </si>
+  <si>
+    <t>calle 152 #96a-39</t>
+  </si>
+  <si>
+    <t>FXXI0011</t>
+  </si>
+  <si>
+    <t>Esneider Palacios Marin</t>
+  </si>
+  <si>
+    <t>Cr 102 A N 131 B 29</t>
+  </si>
+  <si>
+    <t>XDSG0020</t>
+  </si>
+  <si>
+    <t>9F</t>
+  </si>
+  <si>
+    <t>Jonathan andres díaz bustos</t>
+  </si>
+  <si>
+    <t>calle 74 #71-70</t>
+  </si>
+  <si>
+    <t>Verónica Alexandra Arteaga Beltrán</t>
+  </si>
+  <si>
+    <t>Carrera 69D #24-15</t>
+  </si>
+  <si>
+    <t>XDSG0034</t>
+  </si>
+  <si>
+    <t>7D</t>
+  </si>
+  <si>
+    <t>Valerie Tirado</t>
+  </si>
+  <si>
+    <t>Av Las Americas #33-50</t>
+  </si>
+  <si>
+    <t>ACS01281</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>Carlos Saenz</t>
+  </si>
+  <si>
+    <t>Carrera 57 #22 a 41</t>
+  </si>
+  <si>
+    <t>FUSG0060</t>
+  </si>
+  <si>
+    <t>7C</t>
+  </si>
+  <si>
+    <t>german martinez</t>
+  </si>
+  <si>
+    <t>Carrera 54 #18 sur-30</t>
+  </si>
+  <si>
+    <t>GWA2-44-30_AS02</t>
+  </si>
+  <si>
+    <t>JENNY SUARE</t>
+  </si>
+  <si>
+    <t>Carrera 27 #50-58</t>
+  </si>
+  <si>
+    <t>DWHW0003</t>
+  </si>
+  <si>
+    <t>Charles Cardenas</t>
+  </si>
+  <si>
+    <t>Calle 10 #80F-40</t>
+  </si>
+  <si>
+    <t>ASD00840</t>
+  </si>
+  <si>
+    <t>Alejandro Sanchez</t>
+  </si>
+  <si>
+    <t>carrera 14 #152-79</t>
+  </si>
+  <si>
+    <t>ACEC0014</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
+    <t>Juan Mendez</t>
+  </si>
+  <si>
+    <t>Calle 112 #14-47</t>
+  </si>
+  <si>
+    <t>Carlos Andres Becerra</t>
+  </si>
+  <si>
+    <t>Calle 122 #52-57</t>
+  </si>
+  <si>
+    <t>ESXI0002</t>
+  </si>
+  <si>
+    <t>Ignacio Salcedo</t>
+  </si>
+  <si>
+    <t>Calle 89 #76a-03</t>
+  </si>
+  <si>
+    <t>Andres Aranguren</t>
+  </si>
+  <si>
+    <t>Calle 142 #12B-35</t>
+  </si>
+  <si>
+    <t>LUIS_LANCHEROS</t>
+  </si>
+  <si>
+    <t>Luis Eduardo Lancheros</t>
+  </si>
+  <si>
+    <t>Calle 145 # 15 - 53 Apto 406</t>
   </si>
 </sst>
 </file>
@@ -771,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD114"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,13 +1141,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40317700413</v>
+        <v>40323572887</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -832,18 +1156,18 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40317696854</v>
+        <v>40323567806</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -852,18 +1176,18 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40317691488</v>
+        <v>40323259589</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -872,18 +1196,18 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40317605804</v>
+        <v>40323166240</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -892,18 +1216,18 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40317529633</v>
+        <v>40323040454</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -912,18 +1236,18 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40317479749</v>
+        <v>40323024272</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -932,18 +1256,18 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40316841061</v>
+        <v>40322524589</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -952,18 +1276,18 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40316830437</v>
+        <v>40322088550</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -972,18 +1296,18 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40316455848</v>
+        <v>40322086490</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -992,18 +1316,18 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40316213857</v>
+        <v>40321775737</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1012,18 +1336,18 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40316195365</v>
+        <v>40321761725</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1032,18 +1356,18 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40316124521</v>
+        <v>40321569264</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1052,18 +1376,18 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>100008308</v>
+        <v>40321512121</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1072,7 +1396,647 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40321308778</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40321247379</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>40321244602</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>40321231282</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40321178666</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40320907760</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>40320530243</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>40320442007</v>
+      </c>
+      <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>40320181483</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>40320004244</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>40319853553</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>40319733517</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40319485443</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>40319470611</v>
+      </c>
+      <c r="B28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>40319365766</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>40319326279</v>
+      </c>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>40319284933</v>
+      </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>40319071253</v>
+      </c>
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>40319022662</v>
+      </c>
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>40318918755</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>40318503141</v>
+      </c>
+      <c r="B35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>40318443356</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>40318327945</v>
+      </c>
+      <c r="B37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>40318035656</v>
+      </c>
+      <c r="B38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>40317987654</v>
+      </c>
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40324250109</v>
+      </c>
+      <c r="B40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40324110530</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40324045462</v>
+      </c>
+      <c r="B42" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40323888538</v>
+      </c>
+      <c r="B43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>40323765617</v>
+      </c>
+      <c r="B44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>40323748890</v>
+      </c>
+      <c r="B45" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>100008309</v>
+      </c>
+      <c r="B46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1084,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I14"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,13 +2069,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40317700413</v>
+        <v>40323572887</v>
       </c>
       <c r="B2">
-        <v>4271228271</v>
+        <v>4277877902</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1120,30 +2084,30 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J2">
-        <v>40317700413</v>
+        <v>40323572887</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40317696854</v>
+        <v>40323567806</v>
       </c>
       <c r="B3">
-        <v>4271221541</v>
+        <v>4277880750</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1152,30 +2116,30 @@
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J3">
-        <v>40317696854</v>
+        <v>40323567806</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40317691488</v>
+        <v>40323259589</v>
       </c>
       <c r="B4">
-        <v>4271218258</v>
+        <v>4277527670</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1184,30 +2148,30 @@
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J4">
-        <v>40317691488</v>
+        <v>40323259589</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40317605804</v>
+        <v>40323166240</v>
       </c>
       <c r="B5">
-        <v>4271119539</v>
+        <v>4277423396</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1216,30 +2180,30 @@
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="J5">
-        <v>40317605804</v>
+        <v>40323166240</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40317529633</v>
+        <v>40323040454</v>
       </c>
       <c r="B6">
-        <v>4271032951</v>
+        <v>4277274625</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1248,30 +2212,30 @@
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="J6">
-        <v>40317529633</v>
+        <v>40323040454</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40317479749</v>
+        <v>40323024272</v>
       </c>
       <c r="B7">
-        <v>4270978937</v>
+        <v>4277259732</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1280,30 +2244,30 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="J7">
-        <v>40317479749</v>
+        <v>40323024272</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40316841061</v>
+        <v>40322524589</v>
       </c>
       <c r="B8">
-        <v>4270248701</v>
+        <v>4276680886</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1312,30 +2276,30 @@
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J8">
-        <v>40316841061</v>
+        <v>40322524589</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40316830437</v>
+        <v>40322088550</v>
       </c>
       <c r="B9">
-        <v>4270240840</v>
+        <v>4276189748</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1344,30 +2308,30 @@
         <v>9</v>
       </c>
       <c r="F9" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="J9">
-        <v>40316830437</v>
+        <v>40322088550</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40316455848</v>
+        <v>40322086490</v>
       </c>
       <c r="B10">
-        <v>4269817874</v>
+        <v>4276189302</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1376,30 +2340,30 @@
         <v>9</v>
       </c>
       <c r="F10" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="J10">
-        <v>40316455848</v>
+        <v>40322086490</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40316213857</v>
+        <v>40321775737</v>
       </c>
       <c r="B11">
-        <v>4269541997</v>
+        <v>4275834035</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1408,30 +2372,30 @@
         <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J11">
-        <v>40316213857</v>
+        <v>40321775737</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40316195365</v>
+        <v>40321761725</v>
       </c>
       <c r="B12">
-        <v>4269524164</v>
+        <v>4275814852</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1440,30 +2404,30 @@
         <v>9</v>
       </c>
       <c r="F12" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="J12">
-        <v>40316195365</v>
+        <v>40321761725</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40316124521</v>
+        <v>40321569264</v>
       </c>
       <c r="B13">
-        <v>4269441491</v>
+        <v>4275589715</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1472,30 +2436,30 @@
         <v>9</v>
       </c>
       <c r="F13" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="J13">
-        <v>40316124521</v>
+        <v>40321569264</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>100008308</v>
+        <v>40321512121</v>
       </c>
       <c r="B14">
-        <v>4168110107</v>
+        <v>4275531138</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1504,121 +2468,1049 @@
         <v>9</v>
       </c>
       <c r="F14" s="3">
-        <v>44195</v>
+        <v>44200</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="J14">
-        <v>100008308</v>
+        <v>40321512121</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F15" s="3"/>
+      <c r="A15">
+        <v>40321308778</v>
+      </c>
+      <c r="B15">
+        <v>4275296398</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15">
+        <v>40321308778</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40321247379</v>
+      </c>
+      <c r="B16">
+        <v>4275225457</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16">
+        <v>40321247379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>40321244602</v>
+      </c>
+      <c r="B17">
+        <v>4275220882</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17">
+        <v>40321244602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>40321231282</v>
+      </c>
+      <c r="B18">
+        <v>4275207238</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18">
+        <v>40321231282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40321178666</v>
+      </c>
+      <c r="B19">
+        <v>4275150046</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19">
+        <v>40321178666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40320907760</v>
+      </c>
+      <c r="B20">
+        <v>4274838076</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20">
+        <v>40320907760</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>40320530243</v>
+      </c>
+      <c r="B21">
+        <v>4274410102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21">
+        <v>40320530243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>40320442007</v>
+      </c>
+      <c r="B22">
+        <v>4274313082</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22">
+        <v>40320442007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>40320181483</v>
+      </c>
+      <c r="B23">
+        <v>4274008645</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23">
+        <v>40320181483</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>40320004244</v>
+      </c>
+      <c r="B24">
+        <v>4273809044</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24" t="s">
+        <v>106</v>
+      </c>
+      <c r="J24">
+        <v>40320004244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>40319853553</v>
+      </c>
+      <c r="B25">
+        <v>4273638071</v>
+      </c>
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J25">
+        <v>40319853553</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>40319733517</v>
+      </c>
+      <c r="B26">
+        <v>4273503043</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" t="s">
+        <v>111</v>
+      </c>
+      <c r="J26">
+        <v>40319733517</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40319485443</v>
+      </c>
+      <c r="B27">
+        <v>4273227374</v>
+      </c>
+      <c r="C27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" t="s">
+        <v>114</v>
+      </c>
+      <c r="J27">
+        <v>40319485443</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>40319470611</v>
+      </c>
+      <c r="B28">
+        <v>4273212268</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" t="s">
+        <v>116</v>
+      </c>
+      <c r="J28">
+        <v>40319470611</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>40319365766</v>
+      </c>
+      <c r="B29">
+        <v>4273098053</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" t="s">
+        <v>118</v>
+      </c>
+      <c r="J29">
+        <v>40319365766</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>40319326279</v>
+      </c>
+      <c r="B30">
+        <v>4273050884</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G30" t="s">
+        <v>120</v>
+      </c>
+      <c r="H30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I30" t="s">
+        <v>122</v>
+      </c>
+      <c r="J30">
+        <v>40319326279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>40319284933</v>
+      </c>
+      <c r="B31">
+        <v>4273006099</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J31">
+        <v>40319284933</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>40319071253</v>
+      </c>
+      <c r="B32">
+        <v>4272764274</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>125</v>
+      </c>
+      <c r="I32" t="s">
+        <v>126</v>
+      </c>
+      <c r="J32">
+        <v>40319071253</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>40319022662</v>
+      </c>
+      <c r="B33">
+        <v>4272708257</v>
+      </c>
+      <c r="C33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G33" t="s">
+        <v>98</v>
+      </c>
+      <c r="H33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" t="s">
+        <v>129</v>
+      </c>
+      <c r="J33">
+        <v>40319022662</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>40318918755</v>
+      </c>
+      <c r="B34">
+        <v>4272590606</v>
+      </c>
+      <c r="C34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" t="s">
+        <v>132</v>
+      </c>
+      <c r="I34" t="s">
+        <v>133</v>
+      </c>
+      <c r="J34">
+        <v>40318918755</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>40318503141</v>
+      </c>
+      <c r="B35">
+        <v>4272122449</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" t="s">
+        <v>134</v>
+      </c>
+      <c r="I35" t="s">
+        <v>135</v>
+      </c>
+      <c r="J35">
+        <v>40318503141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>40318443356</v>
+      </c>
+      <c r="B36">
+        <v>4272054765</v>
+      </c>
+      <c r="C36" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G36" t="s">
+        <v>137</v>
+      </c>
+      <c r="H36" t="s">
+        <v>138</v>
+      </c>
+      <c r="I36" t="s">
+        <v>139</v>
+      </c>
+      <c r="J36">
+        <v>40318443356</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>40318327945</v>
+      </c>
+      <c r="B37">
+        <v>4271933031</v>
+      </c>
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G37" t="s">
+        <v>141</v>
+      </c>
+      <c r="H37" t="s">
+        <v>142</v>
+      </c>
+      <c r="I37" t="s">
+        <v>143</v>
+      </c>
+      <c r="J37">
+        <v>40318327945</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>40318035656</v>
+      </c>
+      <c r="B38">
+        <v>4271601942</v>
+      </c>
+      <c r="C38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G38" t="s">
+        <v>145</v>
+      </c>
+      <c r="H38" t="s">
+        <v>146</v>
+      </c>
+      <c r="I38" t="s">
+        <v>147</v>
+      </c>
+      <c r="J38">
+        <v>40318035656</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>40317987654</v>
+      </c>
+      <c r="B39">
+        <v>4271552085</v>
+      </c>
+      <c r="C39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" t="s">
+        <v>149</v>
+      </c>
+      <c r="I39" t="s">
+        <v>150</v>
+      </c>
+      <c r="J39">
+        <v>40317987654</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40324250109</v>
+      </c>
+      <c r="B40">
+        <v>4278648382</v>
+      </c>
+      <c r="C40" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G40" t="s">
+        <v>120</v>
+      </c>
+      <c r="H40" t="s">
+        <v>152</v>
+      </c>
+      <c r="I40" t="s">
+        <v>153</v>
+      </c>
+      <c r="J40">
+        <v>40324250109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40324110530</v>
+      </c>
+      <c r="B41">
+        <v>4278489752</v>
+      </c>
+      <c r="C41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G41" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" t="s">
+        <v>155</v>
+      </c>
+      <c r="I41" t="s">
+        <v>156</v>
+      </c>
+      <c r="J41">
+        <v>40324110530</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40324045462</v>
+      </c>
+      <c r="B42">
+        <v>4278408884</v>
+      </c>
+      <c r="C42" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G42" t="s">
+        <v>158</v>
+      </c>
+      <c r="H42" t="s">
+        <v>159</v>
+      </c>
+      <c r="I42" t="s">
+        <v>160</v>
+      </c>
+      <c r="J42">
+        <v>40324045462</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40323888538</v>
+      </c>
+      <c r="B43">
+        <v>4278235522</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G43" t="s">
+        <v>50</v>
+      </c>
+      <c r="H43" t="s">
+        <v>161</v>
+      </c>
+      <c r="I43" t="s">
+        <v>162</v>
+      </c>
+      <c r="J43">
+        <v>40323888538</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>40323765617</v>
+      </c>
+      <c r="B44">
+        <v>4278100517</v>
+      </c>
+      <c r="C44" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G44" t="s">
+        <v>158</v>
+      </c>
+      <c r="H44" t="s">
+        <v>164</v>
+      </c>
+      <c r="I44" t="s">
+        <v>165</v>
+      </c>
+      <c r="J44">
+        <v>40323765617</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>40323748890</v>
+      </c>
+      <c r="B45">
+        <v>4278080950</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G45" t="s">
+        <v>57</v>
+      </c>
+      <c r="H45" t="s">
+        <v>166</v>
+      </c>
+      <c r="I45" t="s">
+        <v>167</v>
+      </c>
+      <c r="J45">
+        <v>40323748890</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>100008309</v>
+      </c>
+      <c r="B46" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="3">
+        <v>44200</v>
+      </c>
+      <c r="G46" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" t="s">
+        <v>169</v>
+      </c>
+      <c r="I46" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46">
+        <v>3007874356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.25">
@@ -1629,48 +3521,6 @@
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizacion de contenidos de index y barra de navegacion
</commit_message>
<xml_diff>
--- a/Files/Temp_os_adm/900987412_3.xlsx
+++ b/Files/Temp_os_adm/900987412_3.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="109">
   <si>
     <t>Nombre Destinatario</t>
   </si>
@@ -200,205 +200,298 @@
     <t>BOGOTA</t>
   </si>
   <si>
-    <t>6E</t>
-  </si>
-  <si>
     <t>11F</t>
   </si>
   <si>
-    <t>3F</t>
-  </si>
-  <si>
     <t>ACCESORIOS CELULAR</t>
   </si>
   <si>
     <t>TA50-BLANCO</t>
   </si>
   <si>
-    <t>XDXI0017</t>
-  </si>
-  <si>
     <t>8D</t>
   </si>
   <si>
-    <t>1F</t>
-  </si>
-  <si>
-    <t>DWSG0009</t>
-  </si>
-  <si>
-    <t>062CS24469</t>
-  </si>
-  <si>
     <t>1A</t>
   </si>
   <si>
-    <t>XDXI0010</t>
-  </si>
-  <si>
-    <t>XDSG0034</t>
-  </si>
-  <si>
-    <t>7D</t>
-  </si>
-  <si>
-    <t>Valerie Tirado</t>
-  </si>
-  <si>
-    <t>Av Las Americas #33-50</t>
-  </si>
-  <si>
-    <t>XDXI0001</t>
-  </si>
-  <si>
     <t>4E</t>
   </si>
   <si>
-    <t>Paul Ramírez</t>
-  </si>
-  <si>
-    <t>Calle 74a #81a-05</t>
-  </si>
-  <si>
-    <t>FXXI0004</t>
-  </si>
-  <si>
-    <t>Hernando Guerrero</t>
-  </si>
-  <si>
-    <t>Carrera 73 #63-90</t>
-  </si>
-  <si>
-    <t>DWSG0002</t>
-  </si>
-  <si>
-    <t>Wilmer Flores</t>
-  </si>
-  <si>
-    <t>Calle 146 #7-b</t>
-  </si>
-  <si>
-    <t>XDSG0001</t>
-  </si>
-  <si>
-    <t>8B</t>
-  </si>
-  <si>
-    <t>iazet saiz</t>
-  </si>
-  <si>
-    <t>diagonal 15 B #104-46</t>
-  </si>
-  <si>
-    <t>FUSG0030</t>
-  </si>
-  <si>
-    <t>9E</t>
-  </si>
-  <si>
-    <t>Javier Arias</t>
-  </si>
-  <si>
-    <t>calle 51 #73a-16</t>
-  </si>
-  <si>
-    <t>FXHW0015</t>
-  </si>
-  <si>
-    <t>Rafael romero</t>
-  </si>
-  <si>
-    <t>Carrera24a#40a-52 #40a-52</t>
-  </si>
-  <si>
-    <t>Miguel Angel Cardenas Lugo</t>
-  </si>
-  <si>
-    <t>Carrera 100 #17 a-27</t>
-  </si>
-  <si>
-    <t>FMAP0003</t>
-  </si>
-  <si>
-    <t>7F</t>
-  </si>
-  <si>
-    <t>Juan Camilo Ordoñez</t>
-  </si>
-  <si>
-    <t>Calle 49 #6-39</t>
-  </si>
-  <si>
-    <t>FUSG0053</t>
-  </si>
-  <si>
     <t>2D</t>
   </si>
   <si>
-    <t>Ricardo Berrío</t>
-  </si>
-  <si>
-    <t>Carrera 8a #106-00</t>
-  </si>
-  <si>
-    <t>FUSG0003</t>
-  </si>
-  <si>
-    <t>5C</t>
-  </si>
-  <si>
-    <t>Pablo Gamm</t>
-  </si>
-  <si>
-    <t>Carrera 21 #133-85</t>
-  </si>
-  <si>
-    <t>Jonnathan Jimen</t>
-  </si>
-  <si>
-    <t>Carrera 80 bis #7A-15</t>
-  </si>
-  <si>
-    <t>Jose Ignacio García</t>
-  </si>
-  <si>
-    <t>Cra 58C #144-15</t>
-  </si>
-  <si>
-    <t>ADAP0007</t>
-  </si>
-  <si>
-    <t>1G</t>
-  </si>
-  <si>
-    <t>Tabitha Wells</t>
-  </si>
-  <si>
-    <t>Carrera 1 Este #72a-96</t>
-  </si>
-  <si>
-    <t>FERNANDO MORENO</t>
-  </si>
-  <si>
-    <t>Diagonal 82 bis #85 -21</t>
-  </si>
-  <si>
-    <t>ASSG0002</t>
-  </si>
-  <si>
-    <t>3E</t>
-  </si>
-  <si>
-    <t>Daniel Almánzar</t>
-  </si>
-  <si>
-    <t>Carrera 10 # 84c - 35 Apartamento 301</t>
-  </si>
-  <si>
-    <t>Jose Melo</t>
-  </si>
-  <si>
-    <t>calle 4 #73-31</t>
+    <t>075CS27129</t>
+  </si>
+  <si>
+    <t>Santiago zambrano</t>
+  </si>
+  <si>
+    <t>Calle 106 A #48-21</t>
+  </si>
+  <si>
+    <t>FXXI0021</t>
+  </si>
+  <si>
+    <t>6F</t>
+  </si>
+  <si>
+    <t>Luis Fernando León Quiroga</t>
+  </si>
+  <si>
+    <t>Carrera 16 A #48-40</t>
+  </si>
+  <si>
+    <t>ACFI0008</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>Gustavo Hernández</t>
+  </si>
+  <si>
+    <t>carrera 20 #184-48</t>
+  </si>
+  <si>
+    <t>FXXI0010</t>
+  </si>
+  <si>
+    <t>8F</t>
+  </si>
+  <si>
+    <t>Victor Sotelo</t>
+  </si>
+  <si>
+    <t>Calle 44 Sur No 21-73 Santa Lucía 4</t>
+  </si>
+  <si>
+    <t>FXXI0009</t>
+  </si>
+  <si>
+    <t>NESTOR AGUILAR</t>
+  </si>
+  <si>
+    <t>Carrera 102 #20-37</t>
+  </si>
+  <si>
+    <t>AGL01467</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>Juan Sebastián Murcia</t>
+  </si>
+  <si>
+    <t>Calle 89 #13A-57</t>
+  </si>
+  <si>
+    <t>IGSG0023</t>
+  </si>
+  <si>
+    <t>0F</t>
+  </si>
+  <si>
+    <t>Anderson Sandoval</t>
+  </si>
+  <si>
+    <t>Avenida el dorado #69A-51</t>
+  </si>
+  <si>
+    <t>FXXI0027</t>
+  </si>
+  <si>
+    <t>5E</t>
+  </si>
+  <si>
+    <t>Indira alba Lucía Arevalo</t>
+  </si>
+  <si>
+    <t>carrera 7g # 152a -24</t>
+  </si>
+  <si>
+    <t>FUSG0060</t>
+  </si>
+  <si>
+    <t>7C</t>
+  </si>
+  <si>
+    <t>juan david parra</t>
+  </si>
+  <si>
+    <t>calle 127a #53a-68</t>
+  </si>
+  <si>
+    <t>FUSG0001</t>
+  </si>
+  <si>
+    <t>9D</t>
+  </si>
+  <si>
+    <t>jairo botero</t>
+  </si>
+  <si>
+    <t>Calle 40 sur #78A-12</t>
+  </si>
+  <si>
+    <t>XDHW0007</t>
+  </si>
+  <si>
+    <t>5F</t>
+  </si>
+  <si>
+    <t>Miguel Rojas</t>
+  </si>
+  <si>
+    <t>Carrera 5 72 A 39</t>
+  </si>
+  <si>
+    <t>OXSG0021</t>
+  </si>
+  <si>
+    <t>3G</t>
+  </si>
+  <si>
+    <t>Carlos Peinado</t>
+  </si>
+  <si>
+    <t>Calle 137 #91-97</t>
+  </si>
+  <si>
+    <t>FUSG0062</t>
+  </si>
+  <si>
+    <t>Sebastián Fernando Mora Rocha</t>
+  </si>
+  <si>
+    <t>Calle 6C #78-32</t>
+  </si>
+  <si>
+    <t>EP-TA20JBEUGUS</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Alexander Vanegas</t>
+  </si>
+  <si>
+    <t>Carrera 49 #94-75</t>
+  </si>
+  <si>
+    <t>057CS22123</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>JUAN ORLANDO CARDENAS</t>
+  </si>
+  <si>
+    <t>Carrera 71 #50-19</t>
+  </si>
+  <si>
+    <t>TA20MICRO-BLANCO</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>Juan C Mancipe</t>
+  </si>
+  <si>
+    <t>Calle 71a #84a-34</t>
+  </si>
+  <si>
+    <t>Luis Alberto Blanco Vera</t>
+  </si>
+  <si>
+    <t>Carrera 46 #141-59</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>Paula Aguilera</t>
+  </si>
+  <si>
+    <t>carrera 69 D #25-45</t>
+  </si>
+  <si>
+    <t>Sofia Buendia</t>
+  </si>
+  <si>
+    <t>Calle 107 #52-49</t>
+  </si>
+  <si>
+    <t>FSAP0005</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>Andres Garces</t>
+  </si>
+  <si>
+    <t>Calle 118 #60-67</t>
+  </si>
+  <si>
+    <t>ESAP0002</t>
+  </si>
+  <si>
+    <t>Tatiana Orozco</t>
+  </si>
+  <si>
+    <t>Carrera 18c #122-40</t>
+  </si>
+  <si>
+    <t>Andres Felipe Rodriguez Perez</t>
+  </si>
+  <si>
+    <t>Carrera 58c #152b-22</t>
+  </si>
+  <si>
+    <t>FUSG0042</t>
+  </si>
+  <si>
+    <t>David Medina Medellin</t>
+  </si>
+  <si>
+    <t>Calle 136 #17a-33</t>
+  </si>
+  <si>
+    <t>FSSG0083</t>
+  </si>
+  <si>
+    <t>7E</t>
+  </si>
+  <si>
+    <t>Nicolás Parra Triviño</t>
+  </si>
+  <si>
+    <t>Carrera 41 #1-62</t>
+  </si>
+  <si>
+    <t>ACEC0012</t>
+  </si>
+  <si>
+    <t>Juan Mendez</t>
+  </si>
+  <si>
+    <t>Calle 112 #14-47</t>
+  </si>
+  <si>
+    <t>ACS00428</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>fernando castiblanco</t>
+  </si>
+  <si>
+    <t>CARRERA 100 A #141-10</t>
   </si>
 </sst>
 </file>
@@ -816,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,13 +955,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40326277454</v>
+        <v>40328887973</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -877,18 +970,18 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40326011981</v>
+        <v>40328885659</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -897,18 +990,18 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40326006941</v>
+        <v>40328793277</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -917,18 +1010,18 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40325898014</v>
+        <v>40328727906</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -937,18 +1030,18 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40325489814</v>
+        <v>40327750694</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -957,18 +1050,18 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40325396133</v>
+        <v>40328674944</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -977,18 +1070,18 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40325137071</v>
+        <v>40328578586</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -997,18 +1090,18 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40325058874</v>
+        <v>40327337669</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1017,18 +1110,18 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40325036135</v>
+        <v>40328552642</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1037,18 +1130,18 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40324911872</v>
+        <v>40328234366</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1057,18 +1150,18 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40324851020</v>
+        <v>40328055720</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1077,18 +1170,18 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40324841798</v>
+        <v>40327914417</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1097,18 +1190,18 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40324815210</v>
+        <v>40327837452</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1117,19 +1210,19 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>100008311</v>
+        <v>40327730996</v>
       </c>
       <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
-        <v>71</v>
-      </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
@@ -1137,18 +1230,18 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>40318443356</v>
+        <v>40327704973</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1157,18 +1250,18 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>100008314</v>
+        <v>40327662486</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -1177,18 +1270,18 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>40326741953</v>
+        <v>40327647965</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -1197,7 +1290,187 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40327626387</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40327585346</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>40327313306</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>40327051556</v>
+      </c>
+      <c r="B22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>40326925982</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>40326879108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>40324951875</v>
+      </c>
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>40324045462</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40329006514</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1209,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I18"/>
+      <selection activeCell="I2" sqref="I2:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,13 +1503,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40326277454</v>
+        <v>40328887973</v>
       </c>
       <c r="B2">
-        <v>4280949190</v>
+        <v>4283871696</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1245,30 +1518,30 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J2">
-        <v>40326277454</v>
+        <v>40328887973</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40326011981</v>
+        <v>40328885659</v>
       </c>
       <c r="B3">
-        <v>4280647980</v>
+        <v>4283871479</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1277,30 +1550,30 @@
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J3">
-        <v>40326011981</v>
+        <v>40328885659</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40326006941</v>
+        <v>40328793277</v>
       </c>
       <c r="B4">
-        <v>4280643269</v>
+        <v>4283771281</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1309,30 +1582,30 @@
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
       <c r="J4">
-        <v>40326006941</v>
+        <v>40328793277</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40325898014</v>
+        <v>40328727906</v>
       </c>
       <c r="B5">
-        <v>4280520952</v>
+        <v>4283700277</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1341,30 +1614,30 @@
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J5">
-        <v>40325898014</v>
+        <v>40328727906</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40325489814</v>
+        <v>40327750694</v>
       </c>
       <c r="B6">
-        <v>4280043311</v>
+        <v>4282599679</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1373,30 +1646,30 @@
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="J6">
-        <v>40325489814</v>
+        <v>40327750694</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40325396133</v>
+        <v>40328674944</v>
       </c>
       <c r="B7">
-        <v>4279939039</v>
+        <v>4283640285</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1405,30 +1678,30 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
         <v>38</v>
       </c>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="J7">
-        <v>40325396133</v>
+        <v>40328674944</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40325137071</v>
+        <v>40328578586</v>
       </c>
       <c r="B8">
-        <v>4279637890</v>
+        <v>4283533175</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1437,30 +1710,30 @@
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J8">
-        <v>40325137071</v>
+        <v>40328578586</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40325058874</v>
+        <v>40327337669</v>
       </c>
       <c r="B9">
-        <v>4279560113</v>
+        <v>4282137833</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1469,30 +1742,30 @@
         <v>9</v>
       </c>
       <c r="F9" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J9">
-        <v>40325058874</v>
+        <v>40327337669</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40325036135</v>
+        <v>40328552642</v>
       </c>
       <c r="B10">
-        <v>4279532521</v>
+        <v>4283504151</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1501,30 +1774,30 @@
         <v>9</v>
       </c>
       <c r="F10" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J10">
-        <v>40325036135</v>
+        <v>40328552642</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40324911872</v>
+        <v>40328234366</v>
       </c>
       <c r="B11">
-        <v>4279394430</v>
+        <v>4283147507</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1533,30 +1806,30 @@
         <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J11">
-        <v>40324911872</v>
+        <v>40328234366</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40324851020</v>
+        <v>40328055720</v>
       </c>
       <c r="B12">
-        <v>4279327223</v>
+        <v>4282955765</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1565,30 +1838,30 @@
         <v>9</v>
       </c>
       <c r="F12" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J12">
-        <v>40324851020</v>
+        <v>40328055720</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40324841798</v>
+        <v>40327914417</v>
       </c>
       <c r="B13">
-        <v>4279313700</v>
+        <v>4282785477</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1597,62 +1870,62 @@
         <v>9</v>
       </c>
       <c r="F13" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J13">
-        <v>40324841798</v>
+        <v>40327914417</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40324815210</v>
+        <v>40327837452</v>
       </c>
       <c r="B14">
-        <v>4279284661</v>
+        <v>4282699048</v>
       </c>
       <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" t="s">
         <v>66</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="3">
-        <v>44201</v>
-      </c>
-      <c r="G14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" t="s">
-        <v>69</v>
-      </c>
       <c r="J14">
-        <v>40324815210</v>
+        <v>40327837452</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>100008311</v>
+        <v>40327730996</v>
       </c>
       <c r="B15">
-        <v>4268191532</v>
+        <v>4282579091</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1661,30 +1934,30 @@
         <v>9</v>
       </c>
       <c r="F15" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="H15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" t="s">
         <v>70</v>
       </c>
-      <c r="I15" t="s">
-        <v>71</v>
-      </c>
       <c r="J15">
-        <v>100008311</v>
+        <v>40327730996</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>40318443356</v>
+        <v>40327704973</v>
       </c>
       <c r="B16">
-        <v>4272054765</v>
+        <v>4282549341</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1693,30 +1966,30 @@
         <v>9</v>
       </c>
       <c r="F16" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="J16">
-        <v>40318443356</v>
+        <v>40327704973</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>100008314</v>
+        <v>40327662486</v>
       </c>
       <c r="B17">
-        <v>1771</v>
+        <v>4282497941</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1725,30 +1998,30 @@
         <v>9</v>
       </c>
       <c r="F17" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J17">
-        <v>100008314</v>
+        <v>40327662486</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>40326741953</v>
+        <v>40327647965</v>
       </c>
       <c r="B18">
-        <v>4281473042</v>
+        <v>4282485355</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1757,47 +2030,308 @@
         <v>9</v>
       </c>
       <c r="F18" s="3">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J18">
-        <v>40326741953</v>
+        <v>40327647965</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
+      <c r="A19">
+        <v>40327626387</v>
+      </c>
+      <c r="B19">
+        <v>4282451969</v>
+      </c>
+      <c r="C19">
+        <v>905879</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19">
+        <v>40327626387</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
+      <c r="A20">
+        <v>40327585346</v>
+      </c>
+      <c r="B20">
+        <v>4282418136</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20">
+        <v>40327585346</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="3"/>
+      <c r="A21">
+        <v>40327313306</v>
+      </c>
+      <c r="B21">
+        <v>4282112090</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21">
+        <v>40327313306</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
+      <c r="A22">
+        <v>40327051556</v>
+      </c>
+      <c r="B22">
+        <v>4281817462</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22">
+        <v>40327051556</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
+      <c r="A23">
+        <v>40326925982</v>
+      </c>
+      <c r="B23">
+        <v>4281678200</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J23">
+        <v>40326925982</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="3"/>
+      <c r="A24">
+        <v>40326879108</v>
+      </c>
+      <c r="B24">
+        <v>4281626085</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24">
+        <v>40326879108</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="3"/>
+      <c r="A25">
+        <v>40324951875</v>
+      </c>
+      <c r="B25">
+        <v>4279438680</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" t="s">
+        <v>100</v>
+      </c>
+      <c r="I25" t="s">
+        <v>101</v>
+      </c>
+      <c r="J25">
+        <v>40324951875</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
+      <c r="A26">
+        <v>40324045462</v>
+      </c>
+      <c r="B26">
+        <v>4278408884</v>
+      </c>
+      <c r="C26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" t="s">
+        <v>103</v>
+      </c>
+      <c r="I26" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26">
+        <v>40324045462</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
+      <c r="A27">
+        <v>40329006514</v>
+      </c>
+      <c r="B27">
+        <v>40329006514</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="3">
+        <v>44202</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" t="s">
+        <v>108</v>
+      </c>
+      <c r="J27">
+        <v>40329006514</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
@@ -1846,21 +2380,6 @@
     </row>
     <row r="43" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correccion de error al guardar os
</commit_message>
<xml_diff>
--- a/Files/Temp_os_adm/900987412_3.xlsx
+++ b/Files/Temp_os_adm/900987412_3.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="80">
   <si>
     <t>Nombre Destinatario</t>
   </si>
@@ -203,145 +203,208 @@
     <t>ACCESORIOS CELULAR</t>
   </si>
   <si>
-    <t>7B</t>
+    <t>7D</t>
+  </si>
+  <si>
+    <t>11D</t>
+  </si>
+  <si>
+    <t>EP-DG950CBE-BULK</t>
+  </si>
+  <si>
+    <t>EP-TA20JBEUGUS</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>TA50-BLANCO</t>
+  </si>
+  <si>
+    <t>11F</t>
+  </si>
+  <si>
+    <t>XDXI0003</t>
+  </si>
+  <si>
+    <t>5D</t>
+  </si>
+  <si>
+    <t>ACFI0008</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>gabriel tochoy</t>
+  </si>
+  <si>
+    <t>calle 27sur #29B-20</t>
+  </si>
+  <si>
+    <t>XDXI0017</t>
+  </si>
+  <si>
+    <t>8D</t>
+  </si>
+  <si>
+    <t>Edwin Martínez</t>
+  </si>
+  <si>
+    <t>Carrera 8 172A 85</t>
+  </si>
+  <si>
+    <t>jakelin pintor</t>
+  </si>
+  <si>
+    <t>Calle 147 #15-81</t>
+  </si>
+  <si>
+    <t>Edward Cifuentes</t>
+  </si>
+  <si>
+    <t>Calle 139 #98c-16</t>
+  </si>
+  <si>
+    <t>FMAP0003</t>
+  </si>
+  <si>
+    <t>7F</t>
+  </si>
+  <si>
+    <t>mateo tellez</t>
+  </si>
+  <si>
+    <t>calle 35 sur #69 a-22</t>
+  </si>
+  <si>
+    <t>FXXI0009</t>
+  </si>
+  <si>
+    <t>Jenny Moreno</t>
+  </si>
+  <si>
+    <t>Transversal 76 #82C-6</t>
+  </si>
+  <si>
+    <t>Ana María Joves Jaramillo</t>
+  </si>
+  <si>
+    <t>Calle 127 #87A-24</t>
+  </si>
+  <si>
+    <t>057CS22123</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>Juan Felipe Cabrera Silva</t>
+  </si>
+  <si>
+    <t>Cra 12 #110-79</t>
+  </si>
+  <si>
+    <t>Alberto García</t>
+  </si>
+  <si>
+    <t>calle 113 #56-24</t>
+  </si>
+  <si>
+    <t>FUSG0048</t>
+  </si>
+  <si>
+    <t>8B</t>
+  </si>
+  <si>
+    <t>Erika Perez</t>
+  </si>
+  <si>
+    <t>Calle 151 #54A-41</t>
+  </si>
+  <si>
+    <t>Jeisson González</t>
+  </si>
+  <si>
+    <t>Calle 69 Sur #78-27</t>
+  </si>
+  <si>
+    <t>OXAP0017</t>
+  </si>
+  <si>
+    <t>Cristian Escarraga</t>
+  </si>
+  <si>
+    <t>Cra 15a #106-15</t>
+  </si>
+  <si>
+    <t>Camilo Díaz</t>
+  </si>
+  <si>
+    <t>Transversal 78B #40 G-43 SUR</t>
+  </si>
+  <si>
+    <t>ESSG0016</t>
+  </si>
+  <si>
+    <t>2F</t>
+  </si>
+  <si>
+    <t>Leonardo Ruiz</t>
+  </si>
+  <si>
+    <t>Cra 118 #86-20</t>
+  </si>
+  <si>
+    <t>Patricia Londoño</t>
+  </si>
+  <si>
+    <t>Carrera 66 #23 A 42</t>
   </si>
   <si>
     <t>FUSG0059</t>
   </si>
   <si>
-    <t>7D</t>
-  </si>
-  <si>
-    <t>11D</t>
-  </si>
-  <si>
-    <t>EP-DG950CBE-BULK</t>
-  </si>
-  <si>
-    <t>066CS24808</t>
-  </si>
-  <si>
-    <t>3C</t>
-  </si>
-  <si>
-    <t>Alex Zapata</t>
-  </si>
-  <si>
-    <t>carrera 3 #9-17</t>
-  </si>
-  <si>
-    <t>065GL24540</t>
-  </si>
-  <si>
-    <t>10F</t>
-  </si>
-  <si>
-    <t>Catalina Jaramillo</t>
-  </si>
-  <si>
-    <t>Carrera 14 #88-31</t>
-  </si>
-  <si>
-    <t>GREIS PAOLA SINNING</t>
-  </si>
-  <si>
-    <t>Calle 164b #4-75</t>
-  </si>
-  <si>
-    <t>FUSG0042</t>
-  </si>
-  <si>
-    <t>4E</t>
-  </si>
-  <si>
-    <t>Santiago Muñoz Correa</t>
-  </si>
-  <si>
-    <t>Calle 59 #45-20</t>
-  </si>
-  <si>
-    <t>OXAP0019</t>
-  </si>
-  <si>
-    <t>1D</t>
-  </si>
-  <si>
-    <t>PAULA DOMINGUEZ</t>
-  </si>
-  <si>
-    <t>Carrera 17 #135-54</t>
-  </si>
-  <si>
-    <t>Gilberto Castellanos</t>
-  </si>
-  <si>
-    <t>Calle 144 #12-68</t>
-  </si>
-  <si>
-    <t>Matías Laverde Huertas</t>
-  </si>
-  <si>
-    <t>Calle 145 #7f-37</t>
-  </si>
-  <si>
-    <t>Estefania jimenez</t>
-  </si>
-  <si>
-    <t>Calle 49 H #10 A-22</t>
-  </si>
-  <si>
-    <t>BASG0009</t>
-  </si>
-  <si>
-    <t>5B</t>
-  </si>
-  <si>
-    <t>Erik Betancourt Mora</t>
-  </si>
-  <si>
-    <t>Cra 68b #00-28</t>
-  </si>
-  <si>
-    <t>ACS00754</t>
-  </si>
-  <si>
-    <t>CESAR AUGUSTO REND</t>
-  </si>
-  <si>
-    <t>Carrera 7 #111-75-402</t>
-  </si>
-  <si>
-    <t>EP-TA20JBEUGUS</t>
-  </si>
-  <si>
-    <t>3D</t>
-  </si>
-  <si>
-    <t>John Denis Durango</t>
-  </si>
-  <si>
-    <t>Cra 11A #191-28</t>
-  </si>
-  <si>
-    <t>ASD00542</t>
-  </si>
-  <si>
-    <t>Juan Rojas</t>
-  </si>
-  <si>
-    <t>Calle 136 #17a-34</t>
-  </si>
-  <si>
-    <t>XDSG0025</t>
-  </si>
-  <si>
-    <t>9E</t>
-  </si>
-  <si>
-    <t>Daniel Rivera</t>
-  </si>
-  <si>
-    <t>carrera 21 #133-85</t>
+    <t>JUAN DAVID MELENDEZ MOLANO</t>
+  </si>
+  <si>
+    <t>Calle 149 #48-16</t>
+  </si>
+  <si>
+    <t>ADSG0025</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>Ivan Dario Sierra</t>
+  </si>
+  <si>
+    <t>Carrera 51 B #16 48-Sur</t>
+  </si>
+  <si>
+    <t>AGL02243</t>
+  </si>
+  <si>
+    <t>11E</t>
+  </si>
+  <si>
+    <t>Fernando Arrazola Jaramillo</t>
+  </si>
+  <si>
+    <t>Calle 80 #9-58</t>
+  </si>
+  <si>
+    <t>XMAP0003</t>
+  </si>
+  <si>
+    <t>7E</t>
+  </si>
+  <si>
+    <t>Ricardo Andrés Rincon Miranda</t>
+  </si>
+  <si>
+    <t>Cll 86 A # 111 A 49</t>
   </si>
 </sst>
 </file>
@@ -759,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:G14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,13 +868,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40332870433</v>
+        <v>40342569819</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -825,13 +888,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40332851586</v>
+        <v>40342546443</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -845,13 +908,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40332786793</v>
+        <v>40342458130</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -865,13 +928,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40332703505</v>
+        <v>40342450266</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -885,13 +948,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40332603491</v>
+        <v>40342422069</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -905,13 +968,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40332495505</v>
+        <v>40342231851</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -925,13 +988,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40332098018</v>
+        <v>40342074188</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -945,13 +1008,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40332005573</v>
+        <v>40341981190</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -965,13 +1028,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40331995846</v>
+        <v>40341755999</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -985,13 +1048,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40331889673</v>
+        <v>40341671536</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1005,13 +1068,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40333129408</v>
+        <v>40340089297</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1025,13 +1088,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40333057521</v>
+        <v>40340944017</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1045,7 +1108,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40333036714</v>
+        <v>40340784827</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
@@ -1060,6 +1123,126 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40340786119</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40342727050</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>40342725360</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>40342975835</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40342956110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40343002348</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1072,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I14"/>
+      <selection activeCell="I2" sqref="I2:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,18 +1271,18 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40332870433</v>
+        <v>40342569819</v>
       </c>
       <c r="B2">
-        <v>4288356285</v>
+        <v>4299346464</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1108,30 +1291,27 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2">
-        <v>40332870433</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>40332851586</v>
+        <v>40342546443</v>
       </c>
       <c r="B3">
-        <v>4288335467</v>
+        <v>4299317867</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1140,30 +1320,27 @@
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3">
-        <v>40332851586</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>40332786793</v>
+        <v>40342458130</v>
       </c>
       <c r="B4">
-        <v>4288261261</v>
+        <v>4299218762</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1172,30 +1349,27 @@
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4">
-        <v>40332786793</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40332703505</v>
+        <v>40342450266</v>
       </c>
       <c r="B5">
-        <v>4288156990</v>
+        <v>4299213159</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1204,30 +1378,27 @@
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5">
-        <v>40332703505</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40332603491</v>
+        <v>40342422069</v>
       </c>
       <c r="B6">
-        <v>4288053950</v>
+        <v>4299176961</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1236,30 +1407,27 @@
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6">
-        <v>40332603491</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40332495505</v>
+        <v>40342231851</v>
       </c>
       <c r="B7">
-        <v>4287939433</v>
+        <v>4298965831</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1268,30 +1436,27 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7">
-        <v>40332495505</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40332098018</v>
+        <v>40342074188</v>
       </c>
       <c r="B8">
-        <v>4287483566</v>
+        <v>4298792478</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1300,30 +1465,27 @@
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8">
-        <v>40332098018</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40332005573</v>
+        <v>40341981190</v>
       </c>
       <c r="B9">
-        <v>4287379551</v>
+        <v>4298695085</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1332,30 +1494,27 @@
         <v>9</v>
       </c>
       <c r="F9" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9">
-        <v>40332005573</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40331995846</v>
+        <v>40341755999</v>
       </c>
       <c r="B10">
-        <v>4287368553</v>
+        <v>4298420227</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1364,30 +1523,27 @@
         <v>9</v>
       </c>
       <c r="F10" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10">
-        <v>40331995846</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40331889673</v>
+        <v>40341671536</v>
       </c>
       <c r="B11">
-        <v>4287248363</v>
+        <v>4298326478</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1396,30 +1552,27 @@
         <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11">
-        <v>40331889673</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>40333129408</v>
+        <v>40340089297</v>
       </c>
       <c r="B12">
-        <v>4288644767</v>
+        <v>4296550035</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1428,30 +1581,27 @@
         <v>9</v>
       </c>
       <c r="F12" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12">
-        <v>40333129408</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40333057521</v>
+        <v>40340944017</v>
       </c>
       <c r="B13">
-        <v>4288566209</v>
+        <v>4297506787</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1460,30 +1610,27 @@
         <v>9</v>
       </c>
       <c r="F13" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13">
-        <v>40333057521</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>40333036714</v>
+        <v>40340784827</v>
       </c>
       <c r="B14">
-        <v>4288543409</v>
+        <v>4297332050</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1492,10 +1639,10 @@
         <v>9</v>
       </c>
       <c r="F14" s="3">
-        <v>44204</v>
+        <v>44209</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="H14" t="s">
         <v>57</v>
@@ -1503,81 +1650,180 @@
       <c r="I14" t="s">
         <v>58</v>
       </c>
-      <c r="J14">
-        <v>40333036714</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40340786119</v>
+      </c>
+      <c r="B15">
+        <v>4297330860</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44209</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40342727050</v>
+      </c>
+      <c r="B16">
+        <v>4299522689</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="3">
+        <v>44209</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>40342725360</v>
+      </c>
+      <c r="B17">
+        <v>4299521608</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44209</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>40342975835</v>
+      </c>
+      <c r="B18">
+        <v>4299802516</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44209</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40342956110</v>
+      </c>
+      <c r="B19">
+        <v>4299779834</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44209</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40343002348</v>
+      </c>
+      <c r="B20">
+        <v>4299834037</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44209</v>
+      </c>
+      <c r="G20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>